<commit_message>
Fixed Minor error in code and updated the 2023 results and leaderboard.
</commit_message>
<xml_diff>
--- a/2023_results.xlsx
+++ b/2023_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b4009995_newcastle_ac_uk/Documents/MEP/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="369" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC4C88D5-6C7E-42D4-AF75-2706A1D48EA5}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8F64262-4D55-4321-9FDD-12B61AE8F7FA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
-  <si>
-    <t>Tricksy Taxonomy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>Round_1</t>
   </si>
@@ -57,9 +54,6 @@
     <t>Final</t>
   </si>
   <si>
-    <t>Of Myths &amp; Monsters</t>
-  </si>
-  <si>
     <t xml:space="preserve">Instructions </t>
   </si>
   <si>
@@ -69,208 +63,211 @@
     <t>Wildcard</t>
   </si>
   <si>
-    <t>Red, In Fur</t>
-  </si>
-  <si>
-    <t>Sea Beasties</t>
-  </si>
-  <si>
-    <t>Mexican Free-Tailed Bat</t>
-  </si>
-  <si>
-    <t>Pride of Lionesses</t>
-  </si>
-  <si>
-    <t>Glaring of Cats</t>
-  </si>
-  <si>
-    <t>Romp of Otters</t>
-  </si>
-  <si>
-    <t>Prickle of Hedgehogs</t>
-  </si>
-  <si>
-    <t>Labor of Moles</t>
-  </si>
-  <si>
-    <t>Sneak of Weasels</t>
-  </si>
-  <si>
-    <t>Conspiracy of Lemurs</t>
-  </si>
-  <si>
-    <t>Lodge of Beavers</t>
-  </si>
-  <si>
-    <t>Troop pf Monkeys</t>
-  </si>
-  <si>
-    <t>Wisdom of Wombats</t>
-  </si>
-  <si>
-    <t>Herd of Reindeer</t>
-  </si>
-  <si>
-    <t>Cauldron of Bats</t>
-  </si>
-  <si>
-    <t>Skulk of Foxes</t>
-  </si>
-  <si>
-    <t>Stench of Skunks</t>
-  </si>
-  <si>
-    <t>Embarrassment of Pandas</t>
-  </si>
-  <si>
-    <t>Town of Prairie Dogs</t>
-  </si>
-  <si>
-    <t>Grizzly Bear</t>
-  </si>
-  <si>
-    <t>Gray Wolf</t>
-  </si>
-  <si>
-    <t>Badger</t>
-  </si>
-  <si>
-    <t>Mountain Lion</t>
-  </si>
-  <si>
-    <t>Kit Fox</t>
-  </si>
-  <si>
-    <t>Jaguar</t>
-  </si>
-  <si>
-    <t>Marsh Rabbit</t>
-  </si>
-  <si>
-    <t>Elk</t>
-  </si>
-  <si>
-    <t>Yellow-Bellied Marmot</t>
-  </si>
-  <si>
-    <t>Black Bear</t>
-  </si>
-  <si>
-    <t>Lined Ground Squirrel</t>
-  </si>
-  <si>
-    <t>Bighorn Sheep</t>
-  </si>
-  <si>
-    <t>Coyote</t>
-  </si>
-  <si>
-    <t>Bison</t>
-  </si>
-  <si>
-    <t>Southern Bog Lemming</t>
-  </si>
-  <si>
-    <t>Orca</t>
-  </si>
-  <si>
-    <t>Common Prawn</t>
-  </si>
-  <si>
-    <t>Olive Sea Snake</t>
-  </si>
-  <si>
-    <t>Hagfish</t>
-  </si>
-  <si>
-    <t>Common Map Turtle</t>
-  </si>
-  <si>
-    <t>Northern Jacena</t>
-  </si>
-  <si>
-    <t>Blanket Octopus</t>
-  </si>
-  <si>
-    <t>Angler Fish</t>
-  </si>
-  <si>
-    <t>Macaroni Penguin</t>
-  </si>
-  <si>
-    <t>Steller's Sea Eagle</t>
-  </si>
-  <si>
-    <t>Arctic Tern</t>
-  </si>
-  <si>
-    <t>Hawaiian Monk Seal</t>
-  </si>
-  <si>
-    <t>Walrus</t>
-  </si>
-  <si>
-    <t>Echidna</t>
-  </si>
-  <si>
-    <t>Ecletu Parrot</t>
-  </si>
-  <si>
-    <t>Dobsonfly</t>
-  </si>
-  <si>
-    <t>Indian Fruit Bat</t>
-  </si>
-  <si>
-    <t>Iberian Ribbed Newt</t>
-  </si>
-  <si>
-    <t>Lichen</t>
-  </si>
-  <si>
-    <t>Muntjac</t>
-  </si>
-  <si>
-    <t>Serval</t>
-  </si>
-  <si>
-    <t>Pangolin</t>
-  </si>
-  <si>
-    <t>Painted Redstart</t>
-  </si>
-  <si>
-    <t>Therapsid</t>
-  </si>
-  <si>
-    <t>Florida Bonneted Bat</t>
-  </si>
-  <si>
-    <t>Lesser NZ Short-tailed Bat</t>
-  </si>
-  <si>
-    <t>Scansoriopterygid</t>
+    <t>Mighty Stripes</t>
+  </si>
+  <si>
+    <t>Itty Bitty Comeback City</t>
+  </si>
+  <si>
+    <t>Animal Engineers</t>
+  </si>
+  <si>
+    <t>Dad Bods</t>
+  </si>
+  <si>
+    <t>Okapi</t>
+  </si>
+  <si>
+    <t>Four-Striped Grass Mouse</t>
+  </si>
+  <si>
+    <t>Striped Polecat</t>
+  </si>
+  <si>
+    <t>Giant-Striped Mongoose</t>
+  </si>
+  <si>
+    <t>Side-Striped Jackal</t>
+  </si>
+  <si>
+    <t>Striped Possum</t>
+  </si>
+  <si>
+    <t>Striped Dolphin</t>
+  </si>
+  <si>
+    <t>Checquered Elephant Shrew</t>
+  </si>
+  <si>
+    <t>Wildcat</t>
+  </si>
+  <si>
+    <t>Highland Tenrec</t>
+  </si>
+  <si>
+    <t>Striped Hyena</t>
+  </si>
+  <si>
+    <t>Fire-Footed Rope Squirrel</t>
+  </si>
+  <si>
+    <t>Striped Rabbit</t>
+  </si>
+  <si>
+    <t>Numbat</t>
+  </si>
+  <si>
+    <t>Kudu</t>
+  </si>
+  <si>
+    <t>Badger bat</t>
+  </si>
+  <si>
+    <t>Shrew Mole</t>
+  </si>
+  <si>
+    <t>Sea Otter</t>
+  </si>
+  <si>
+    <t>Southern Ninguai</t>
+  </si>
+  <si>
+    <t>Grasshopper Mouse</t>
+  </si>
+  <si>
+    <t>Sibree Dwarf Lemur</t>
+  </si>
+  <si>
+    <t>Silver Pika</t>
+  </si>
+  <si>
+    <t>Mara</t>
+  </si>
+  <si>
+    <t>Siberian Chipmunk</t>
+  </si>
+  <si>
+    <t>Itjarijari</t>
+  </si>
+  <si>
+    <t>Silky Anyeater</t>
+  </si>
+  <si>
+    <t>Dik-dik</t>
+  </si>
+  <si>
+    <t>Colo Colo Opossum</t>
+  </si>
+  <si>
+    <t>Bulldog Bat</t>
+  </si>
+  <si>
+    <t>Thor's Hero Shrew</t>
+  </si>
+  <si>
+    <t>Rock Hyrax</t>
+  </si>
+  <si>
+    <t>Pygmy Jerboa</t>
+  </si>
+  <si>
+    <t>Golden Eagle</t>
+  </si>
+  <si>
+    <t>Spongilla Fly</t>
+  </si>
+  <si>
+    <t>Veined Octopus</t>
+  </si>
+  <si>
+    <t>Puffer Fish</t>
+  </si>
+  <si>
+    <t>Palaeocaster</t>
+  </si>
+  <si>
+    <t>Trapdoor Spider</t>
   </si>
   <si>
     <t>Lungfish</t>
   </si>
   <si>
-    <t>Spotted Salamander</t>
-  </si>
-  <si>
-    <t>Hairy Frogfish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hairy Frog </t>
-  </si>
-  <si>
-    <t>Swordfish</t>
-  </si>
-  <si>
-    <t>Leaf Slug</t>
-  </si>
-  <si>
-    <t>Eclectus Parrot</t>
+    <t>Tent-Making Bat</t>
+  </si>
+  <si>
+    <t>Goanna</t>
+  </si>
+  <si>
+    <t>Rufous Hornero</t>
+  </si>
+  <si>
+    <t>Homo habilis</t>
+  </si>
+  <si>
+    <t>Bee</t>
+  </si>
+  <si>
+    <t>Montezuma Oropendola</t>
+  </si>
+  <si>
+    <t>New Caledonian Crow</t>
+  </si>
+  <si>
+    <t>Cathedral Termite</t>
+  </si>
+  <si>
+    <t>Dung Beetle</t>
+  </si>
+  <si>
+    <t>Emperor Penguin</t>
+  </si>
+  <si>
+    <t>Lined Seahorse</t>
+  </si>
+  <si>
+    <t>Owl Monkey</t>
+  </si>
+  <si>
+    <t>Caspian Tern</t>
+  </si>
+  <si>
+    <t>Pacific Spiny Lumpsucker</t>
+  </si>
+  <si>
+    <t>Peacock Wrasse</t>
+  </si>
+  <si>
+    <t>Siamang</t>
+  </si>
+  <si>
+    <t>Darwin's Frog</t>
+  </si>
+  <si>
+    <t>Bat-Eared Fox</t>
+  </si>
+  <si>
+    <t>Spotted Sandpiper</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
+  </si>
+  <si>
+    <t>Giant Water Bug</t>
+  </si>
+  <si>
+    <t>Greater Flamingo</t>
+  </si>
+  <si>
+    <t>Dyak Friut Bat</t>
+  </si>
+  <si>
+    <t>Greater Rhea</t>
+  </si>
+  <si>
+    <t>Three-Spined Stickleback</t>
+  </si>
+  <si>
+    <t>Bumblebee bat</t>
   </si>
 </sst>
 </file>
@@ -643,54 +640,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
         <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">
@@ -698,14 +695,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
         <v>45</v>
       </c>
@@ -713,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
@@ -721,14 +714,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="F3" s="3"/>
+      <c r="N3" s="3"/>
       <c r="P3" s="3" t="s">
         <v>46</v>
       </c>
@@ -743,12 +732,8 @@
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
         <v>47</v>
       </c>
@@ -761,14 +746,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="M5" s="3"/>
       <c r="P5" s="3" t="s">
         <v>48</v>
       </c>
@@ -781,14 +762,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
         <v>49</v>
       </c>
@@ -801,14 +778,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="N7" s="3"/>
       <c r="P7" s="3" t="s">
         <v>50</v>
       </c>
@@ -821,15 +794,11 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="H8" s="1"/>
-      <c r="O8" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
         <v>51</v>
       </c>
@@ -842,14 +811,10 @@
         <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="P9" s="3" t="s">
         <v>52</v>
       </c>
@@ -862,14 +827,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>78</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
         <v>53</v>
       </c>
@@ -882,16 +843,12 @@
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="P11" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="Q11">
         <v>11</v>
@@ -902,16 +859,12 @@
         <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>54</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q12">
         <v>3</v>
@@ -922,17 +875,13 @@
         <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>54</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="M13" s="3"/>
       <c r="N13" s="4"/>
       <c r="P13" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q13">
         <v>14</v>
@@ -943,16 +892,12 @@
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Q14">
         <v>7</v>
@@ -963,16 +908,12 @@
         <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="N15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q15">
         <v>10</v>
@@ -983,16 +924,12 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q16">
         <v>2</v>
@@ -1003,16 +940,12 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
       <c r="P17" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q17">
         <v>15</v>
@@ -1020,21 +953,21 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
         <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
       </c>
       <c r="Q18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1042,40 +975,30 @@
       <c r="D19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="E19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="O19" s="3"/>
       <c r="P19" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Q19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>69</v>
+      <c r="A20" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C20">
         <v>16</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>57</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="N20" s="3"/>
       <c r="P20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q20">
         <v>16</v>
@@ -1088,14 +1011,10 @@
       <c r="D21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="E21" s="3"/>
+      <c r="O21" s="3"/>
       <c r="P21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q21">
         <v>8</v>
@@ -1108,14 +1027,10 @@
       <c r="D22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="G22" s="3"/>
+      <c r="M22" s="3"/>
       <c r="P22" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q22">
         <v>9</v>
@@ -1128,12 +1043,8 @@
       <c r="D23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="E23" s="3"/>
+      <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
         <v>65</v>
       </c>
@@ -1148,14 +1059,10 @@
       <c r="D24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N24" s="3" t="s">
+      <c r="F24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="P24" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="Q24">
         <v>12</v>
@@ -1168,14 +1075,10 @@
       <c r="D25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="E25" s="3"/>
+      <c r="O25" s="3"/>
       <c r="P25" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q25">
         <v>4</v>
@@ -1188,14 +1091,10 @@
       <c r="D26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="H26" s="3"/>
+      <c r="L26" s="3"/>
       <c r="P26" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q26">
         <v>13</v>
@@ -1208,14 +1107,10 @@
       <c r="D27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="E27" s="3"/>
+      <c r="O27" s="3"/>
       <c r="P27" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q27">
         <v>6</v>
@@ -1228,14 +1123,10 @@
       <c r="D28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="F28" s="3"/>
+      <c r="N28" s="3"/>
       <c r="P28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q28">
         <v>11</v>
@@ -1248,14 +1139,10 @@
       <c r="D29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="E29" s="3"/>
+      <c r="O29" s="3"/>
       <c r="P29" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q29">
         <v>3</v>
@@ -1268,15 +1155,11 @@
       <c r="D30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="G30" s="3"/>
       <c r="K30" s="2"/>
-      <c r="M30" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="M30" s="3"/>
       <c r="P30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q30">
         <v>14</v>
@@ -1289,14 +1172,10 @@
       <c r="D31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="E31" s="3"/>
+      <c r="O31" s="3"/>
       <c r="P31" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q31">
         <v>7</v>
@@ -1309,14 +1188,10 @@
       <c r="D32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="F32" s="3"/>
+      <c r="N32" s="3"/>
       <c r="P32" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q32">
         <v>10</v>
@@ -1329,14 +1204,10 @@
       <c r="D33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="E33" s="3"/>
+      <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q33">
         <v>2</v>
@@ -1350,7 +1221,7 @@
         <v>44</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q34">
         <v>15</v>

</xml_diff>

<commit_message>
Updated the results and edited the code so that it works reguardless of the order of the quarters.
</commit_message>
<xml_diff>
--- a/2023_results.xlsx
+++ b/2023_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b4009995_newcastle_ac_uk/Documents/MEP/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="495" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8F64262-4D55-4321-9FDD-12B61AE8F7FA}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFB22A53-3522-4144-B96D-5E77633C9CE2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Round_1</t>
   </si>
@@ -641,7 +641,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -977,7 +977,9 @@
       </c>
       <c r="E19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="O19" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="P19" s="3" t="s">
         <v>61</v>
       </c>
@@ -1012,7 +1014,9 @@
         <v>31</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="O21" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="P21" s="3" t="s">
         <v>63</v>
       </c>
@@ -1044,7 +1048,9 @@
         <v>33</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="O23" s="3"/>
+      <c r="O23" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="P23" s="3" t="s">
         <v>65</v>
       </c>
@@ -1076,7 +1082,9 @@
         <v>35</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="O25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="P25" s="3" t="s">
         <v>67</v>
       </c>
@@ -1108,7 +1116,9 @@
         <v>37</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="O27" s="3"/>
+      <c r="O27" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="P27" s="3" t="s">
         <v>69</v>
       </c>
@@ -1140,7 +1150,9 @@
         <v>39</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="O29" s="3"/>
+      <c r="O29" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="P29" s="3" t="s">
         <v>71</v>
       </c>
@@ -1173,7 +1185,9 @@
         <v>41</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="O31" s="3"/>
+      <c r="O31" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="P31" s="3" t="s">
         <v>73</v>
       </c>
@@ -1205,7 +1219,9 @@
         <v>43</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="O33" s="3"/>
+      <c r="O33" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="P33" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>